<commit_message>
Tests for the Cancellation of an appointment: Failing tests
</commit_message>
<xml_diff>
--- a/docs/PF_TestCases_Cancellation.xlsx
+++ b/docs/PF_TestCases_Cancellation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aaron/PycharmProjects/G89.2022.T21.FP/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A771750C-730F-8640-9E96-C3A56B3AE8AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{029B6136-31AF-5A41-AFE8-916B0A6CD756}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1315,8 +1315,8 @@
   </sheetPr>
   <dimension ref="A1:Z58"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="90" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
Cancel Appointment Function Working Correctly
</commit_message>
<xml_diff>
--- a/docs/PF_TestCases_Cancellation.xlsx
+++ b/docs/PF_TestCases_Cancellation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aaron/PycharmProjects/G89.2022.T21.FP/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{029B6136-31AF-5A41-AFE8-916B0A6CD756}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D4D0FF4-B4A0-384A-953D-7939A4F28F1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-11620" yWindow="-28300" windowWidth="51200" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja 1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="245">
   <si>
     <t>#</t>
   </si>
@@ -53,9 +53,6 @@
   </si>
   <si>
     <t>Valid</t>
-  </si>
-  <si>
-    <t>Case_Valid_01</t>
   </si>
   <si>
     <t>Valid case: Json exists and is correct</t>
@@ -693,9 +690,6 @@
     <t>ced0953d112ab693b83d1ced965fcc670b558235361b9d1bd62536769a1efa3b</t>
   </si>
   <si>
-    <t>Exception: "The format of the JSON file is not valid."</t>
-  </si>
-  <si>
     <t>Exception: "The JSON file is empty"</t>
   </si>
   <si>
@@ -877,13 +871,6 @@
 </t>
   </si>
   <si>
-    <t>{
-"date_signature":"ced0953d112ab693b83d1ced965fcc670b558235361b9d1bd62536769a1efa3b",
-"cancellation_type": "Temporal",
-"reason": "modified"
-}</t>
-  </si>
-  <si>
     <t xml:space="preserve">{
 "date_no_sig":"ced0953d112ab693b83d1ced965fcc670b558235361b9d1bd62536769a1efa3b",
 "cancellation_type": "Temporal",
@@ -953,9 +940,6 @@
   </si>
   <si>
     <t>Case_NV_54</t>
-  </si>
-  <si>
-    <t>Case_NV_55</t>
   </si>
   <si>
     <t>Case_NV_56</t>
@@ -1008,6 +992,25 @@
 "date_signature":"ced0953d112ab693b83d1ced965fcc670b558235361b9d1bd62536769a1efa3b",
 "cancellation_type": "Temporal",
 "reason": "text of the reason""reason": "text of the reason"
+}</t>
+  </si>
+  <si>
+    <t>Valid, Duplication</t>
+  </si>
+  <si>
+    <t>Case_V_55</t>
+  </si>
+  <si>
+    <t>Case_V_01</t>
+  </si>
+  <si>
+    <t>Exception: "JSON Decode Error - Wrong JSON Format"</t>
+  </si>
+  <si>
+    <t>{
+"date_signature":"ced0953d112ab693b83d1ced965fcc670b558235361b9d1bd62536769a1efa3b",
+"cancellation_type": "Temporal",
+"reason": "m"
 }</t>
   </si>
 </sst>
@@ -1315,8 +1318,8 @@
   </sheetPr>
   <dimension ref="A1:Z58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="90" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" topLeftCell="G19" zoomScale="143" workbookViewId="0">
+      <selection activeCell="H57" sqref="H57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -1369,19 +1372,19 @@
         <v>10</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>12</v>
-      </c>
       <c r="G2" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="I2" s="6" t="s">
         <v>160</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1">
@@ -1392,25 +1395,25 @@
         <v>1</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="2" t="s">
-        <v>16</v>
-      </c>
       <c r="G3" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>162</v>
+        <v>243</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1">
@@ -1421,23 +1424,23 @@
         <v>1</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="F4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F4" s="2" t="s">
-        <v>19</v>
-      </c>
       <c r="G4" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H4" s="4"/>
       <c r="I4" s="6" t="s">
-        <v>163</v>
+        <v>243</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1">
@@ -1448,25 +1451,25 @@
         <v>3</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="G5" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="H5" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="G5" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>22</v>
-      </c>
       <c r="I5" s="6" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1">
@@ -1477,25 +1480,25 @@
         <v>3</v>
       </c>
       <c r="C6" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="E6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="F6" s="2" t="s">
-        <v>24</v>
-      </c>
       <c r="G6" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>162</v>
+        <v>243</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1">
@@ -1506,25 +1509,25 @@
         <v>2</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>162</v>
+        <v>243</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="15.75" customHeight="1">
@@ -1535,25 +1538,25 @@
         <v>2</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D8" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="E8" s="6" t="s">
-        <v>28</v>
-      </c>
       <c r="F8" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H8" s="8" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="I8" s="6" t="s">
-        <v>162</v>
+        <v>243</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1">
@@ -1564,25 +1567,25 @@
         <v>2</v>
       </c>
       <c r="C9" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="5" t="s">
-        <v>14</v>
-      </c>
       <c r="E9" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H9" s="8" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I9" s="6" t="s">
-        <v>162</v>
+        <v>243</v>
       </c>
       <c r="J9" s="6"/>
       <c r="K9" s="6"/>
@@ -1610,25 +1613,25 @@
         <v>6</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E10" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F10" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="F10" s="2" t="s">
-        <v>31</v>
-      </c>
       <c r="G10" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H10" s="8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="I10" s="6" t="s">
-        <v>162</v>
+        <v>243</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1">
@@ -1639,25 +1642,25 @@
         <v>6</v>
       </c>
       <c r="C11" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="E11" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="F11" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="F11" s="2" t="s">
-        <v>33</v>
-      </c>
       <c r="G11" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H11" s="8" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I11" s="6" t="s">
-        <v>162</v>
+        <v>243</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1">
@@ -1668,25 +1671,25 @@
         <v>4</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="H12" s="8" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="I12" s="6" t="s">
-        <v>162</v>
+        <v>243</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1">
@@ -1697,25 +1700,25 @@
         <v>4</v>
       </c>
       <c r="C13" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D13" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="E13" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H13" s="8" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="I13" s="6" t="s">
-        <v>162</v>
+        <v>243</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1">
@@ -1726,25 +1729,25 @@
         <v>4</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H14" s="8" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="I14" s="6" t="s">
-        <v>162</v>
+        <v>243</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1">
@@ -1755,25 +1758,25 @@
         <v>12</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H15" s="8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="I15" s="6" t="s">
-        <v>162</v>
+        <v>243</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1">
@@ -1784,25 +1787,25 @@
         <v>12</v>
       </c>
       <c r="C16" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D16" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="E16" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H16" s="8" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I16" s="6" t="s">
-        <v>162</v>
+        <v>243</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="15.75" customHeight="1">
@@ -1813,25 +1816,25 @@
         <v>14</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H17" s="8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="I17" s="6" t="s">
-        <v>162</v>
+        <v>243</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="15.75" customHeight="1">
@@ -1842,25 +1845,25 @@
         <v>14</v>
       </c>
       <c r="C18" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D18" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D18" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="E18" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H18" s="8" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="I18" s="6" t="s">
-        <v>162</v>
+        <v>243</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="15.75" customHeight="1">
@@ -1871,25 +1874,25 @@
         <v>16</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H19" s="8" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I19" s="6" t="s">
-        <v>162</v>
+        <v>243</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="15.75" customHeight="1">
@@ -1900,25 +1903,25 @@
         <v>16</v>
       </c>
       <c r="C20" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D20" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D20" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="E20" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H20" s="8" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="I20" s="6" t="s">
-        <v>162</v>
+        <v>243</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="15.75" customHeight="1">
@@ -1929,25 +1932,25 @@
         <v>18</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H21" s="8" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="I21" s="6" t="s">
-        <v>162</v>
+        <v>243</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="15.75" customHeight="1">
@@ -1958,25 +1961,25 @@
         <v>18</v>
       </c>
       <c r="C22" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D22" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D22" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="E22" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H22" s="8" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="I22" s="6" t="s">
-        <v>162</v>
+        <v>243</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="15.75" customHeight="1">
@@ -1987,25 +1990,25 @@
         <v>20</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H23" s="8" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="I23" s="6" t="s">
-        <v>162</v>
+        <v>243</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="15.75" customHeight="1">
@@ -2016,25 +2019,25 @@
         <v>20</v>
       </c>
       <c r="C24" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D24" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D24" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="E24" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H24" s="8" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="I24" s="6" t="s">
-        <v>162</v>
+        <v>243</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="15.75" customHeight="1">
@@ -2045,25 +2048,25 @@
         <v>22</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H25" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="I25" s="6" t="s">
-        <v>162</v>
+        <v>243</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="15.75" customHeight="1">
@@ -2074,25 +2077,25 @@
         <v>22</v>
       </c>
       <c r="C26" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D26" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D26" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="E26" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H26" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="I26" s="6" t="s">
-        <v>162</v>
+        <v>243</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="15.75" customHeight="1">
@@ -2103,25 +2106,25 @@
         <v>23</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="H27" s="8" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="I27" s="6" t="s">
-        <v>162</v>
+        <v>243</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="15.75" customHeight="1">
@@ -2132,25 +2135,25 @@
         <v>23</v>
       </c>
       <c r="C28" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D28" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D28" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="E28" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="H28" s="8" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="I28" s="6" t="s">
-        <v>162</v>
+        <v>243</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="15.75" customHeight="1">
@@ -2161,25 +2164,25 @@
         <v>23</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="H29" s="7" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="I29" s="6" t="s">
-        <v>162</v>
+        <v>243</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="15.75" customHeight="1">
@@ -2190,25 +2193,25 @@
         <v>7</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="H30" s="7" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="I30" s="6" t="s">
-        <v>162</v>
+        <v>243</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="15.75" customHeight="1">
@@ -2219,25 +2222,25 @@
         <v>7</v>
       </c>
       <c r="C31" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D31" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D31" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="E31" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="H31" s="7" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="I31" s="6" t="s">
-        <v>162</v>
+        <v>243</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="15.75" customHeight="1">
@@ -2248,25 +2251,25 @@
         <v>7</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="H32" s="7" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="I32" s="6" t="s">
-        <v>162</v>
+        <v>243</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="15.75" customHeight="1">
@@ -2277,25 +2280,25 @@
         <v>13</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E33" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="H33" s="7" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="I33" s="6" t="s">
-        <v>162</v>
+        <v>243</v>
       </c>
     </row>
     <row r="34" spans="1:9" ht="15.75" customHeight="1">
@@ -2306,25 +2309,25 @@
         <v>13</v>
       </c>
       <c r="C34" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D34" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D34" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="E34" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="H34" s="7" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="I34" s="6" t="s">
-        <v>162</v>
+        <v>243</v>
       </c>
     </row>
     <row r="35" spans="1:9" ht="15.75" customHeight="1">
@@ -2335,25 +2338,25 @@
         <v>13</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E35" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="H35" s="7" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="I35" s="6" t="s">
-        <v>162</v>
+        <v>243</v>
       </c>
     </row>
     <row r="36" spans="1:9" ht="15.75" customHeight="1">
@@ -2364,25 +2367,25 @@
         <v>24</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E36" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="H36" s="7" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="I36" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="37" spans="1:9" ht="15.75" customHeight="1">
@@ -2393,25 +2396,25 @@
         <v>24</v>
       </c>
       <c r="C37" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D37" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D37" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="E37" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H37" s="7" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="I37" s="6" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="38" spans="1:9" ht="15.75" customHeight="1">
@@ -2422,25 +2425,25 @@
         <v>24</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E38" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H38" s="7" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="I38" s="6" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="39" spans="1:9" ht="15.75" customHeight="1">
@@ -2451,25 +2454,25 @@
         <v>28</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E39" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="H39" s="7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="I39" s="6" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
     </row>
     <row r="40" spans="1:9" ht="15.75" customHeight="1">
@@ -2480,25 +2483,25 @@
         <v>28</v>
       </c>
       <c r="C40" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D40" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D40" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="E40" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H40" s="7" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="I40" s="6" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
     </row>
     <row r="41" spans="1:9" ht="15.75" customHeight="1">
@@ -2509,25 +2512,25 @@
         <v>8</v>
       </c>
       <c r="C41" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D41" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D41" s="6" t="s">
-        <v>14</v>
-      </c>
       <c r="E41" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F41" s="6" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="G41" s="6" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="H41" s="7" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="I41" s="6" t="s">
-        <v>162</v>
+        <v>243</v>
       </c>
     </row>
     <row r="42" spans="1:9" ht="15.75" customHeight="1">
@@ -2538,25 +2541,25 @@
         <v>8</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D42" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E42" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F42" s="6" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="G42" s="6" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="H42" s="7" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="I42" s="6" t="s">
-        <v>162</v>
+        <v>243</v>
       </c>
     </row>
     <row r="43" spans="1:9" ht="15.75" customHeight="1">
@@ -2567,25 +2570,25 @@
         <v>28</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E43" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H43" s="7" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="I43" s="6" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
     </row>
     <row r="44" spans="1:9" ht="15.75" customHeight="1">
@@ -2596,25 +2599,25 @@
         <v>31</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E44" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="H44" s="7" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="I44" s="6" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="45" spans="1:9" ht="15.75" customHeight="1">
@@ -2625,25 +2628,25 @@
         <v>31</v>
       </c>
       <c r="C45" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D45" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D45" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="E45" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="G45" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H45" s="7" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="I45" s="6" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="46" spans="1:9" ht="15.75" customHeight="1">
@@ -2654,25 +2657,25 @@
         <v>31</v>
       </c>
       <c r="C46" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E46" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="G46" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H46" s="7" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="I46" s="6" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="47" spans="1:9" ht="15.75" customHeight="1">
@@ -2683,25 +2686,25 @@
         <v>35</v>
       </c>
       <c r="C47" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E47" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G47" s="2" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="H47" s="7" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="I47" s="6" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
     </row>
     <row r="48" spans="1:9" ht="15.75" customHeight="1">
@@ -2712,25 +2715,25 @@
         <v>35</v>
       </c>
       <c r="C48" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D48" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D48" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="E48" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="G48" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H48" s="7" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I48" s="6" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
     </row>
     <row r="49" spans="1:9" ht="15" customHeight="1">
@@ -2741,25 +2744,25 @@
         <v>35</v>
       </c>
       <c r="C49" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E49" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="G49" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="H49" s="7" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="I49" s="6" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
     </row>
     <row r="50" spans="1:9" ht="15" customHeight="1">
@@ -2770,25 +2773,25 @@
         <v>10</v>
       </c>
       <c r="C50" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D50" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E50" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F50" s="6" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="G50" s="6" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="H50" s="7" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="I50" t="s">
-        <v>162</v>
+        <v>243</v>
       </c>
     </row>
     <row r="51" spans="1:9" ht="15" customHeight="1">
@@ -2799,25 +2802,25 @@
         <v>10</v>
       </c>
       <c r="C51" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D51" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D51" s="6" t="s">
-        <v>14</v>
-      </c>
       <c r="E51" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F51" s="6" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="G51" s="6" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="H51" s="7" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="I51" s="6" t="s">
-        <v>162</v>
+        <v>243</v>
       </c>
     </row>
     <row r="52" spans="1:9" ht="15.75" customHeight="1">
@@ -2828,25 +2831,25 @@
         <v>38</v>
       </c>
       <c r="C52" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E52" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="G52" s="2" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="H52" s="7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I52" s="6" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="53" spans="1:9" ht="15.75" customHeight="1">
@@ -2857,25 +2860,25 @@
         <v>38</v>
       </c>
       <c r="C53" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D53" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D53" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="E53" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="G53" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H53" s="7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I53" s="6" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="54" spans="1:9" ht="14" customHeight="1">
@@ -2886,25 +2889,25 @@
         <v>38</v>
       </c>
       <c r="C54" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E54" s="6" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="G54" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H54" s="7" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="I54" s="6" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="55" spans="1:9" ht="13" customHeight="1">
@@ -2915,25 +2918,25 @@
         <v>42</v>
       </c>
       <c r="C55" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E55" s="6" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="G55" s="2" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="H55" s="7" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="I55" s="6" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
     </row>
     <row r="56" spans="1:9" ht="13" customHeight="1">
@@ -2944,25 +2947,25 @@
         <v>42</v>
       </c>
       <c r="C56" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>14</v>
+        <v>240</v>
       </c>
       <c r="E56" s="6" t="s">
-        <v>230</v>
+        <v>241</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="G56" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H56" s="7" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I56" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
     </row>
     <row r="57" spans="1:9" ht="14" customHeight="1">
@@ -2973,25 +2976,25 @@
         <v>42</v>
       </c>
       <c r="C57" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E57" s="6" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="G57" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H57" s="7" t="s">
-        <v>207</v>
+        <v>244</v>
       </c>
       <c r="I57" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
     </row>
     <row r="58" spans="1:9" ht="13">

</xml_diff>